<commit_message>
update product backlog, add part of sprint 2
</commit_message>
<xml_diff>
--- a/product-backlog.xlsx
+++ b/product-backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WorkDir\McGill-React\homework\Capstone-project\PollsPlanet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAE9E41A-D072-4BB0-A886-8F19752FAD4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8274853-C58F-4673-97A7-6F90E8D8457F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="93">
   <si>
     <t>Team member</t>
   </si>
@@ -264,6 +264,54 @@
   </si>
   <si>
     <t>1. The registered administrator can pass the authorization                   2. The administrator can login into the system</t>
+  </si>
+  <si>
+    <t>Ideal Hours</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>1.5 hrs</t>
+  </si>
+  <si>
+    <t>5 hrs</t>
+  </si>
+  <si>
+    <t>4 hrs</t>
+  </si>
+  <si>
+    <t>2 hrs</t>
+  </si>
+  <si>
+    <t>BK-2.1</t>
+  </si>
+  <si>
+    <t>BK-2.2</t>
+  </si>
+  <si>
+    <t>BK-2.3</t>
+  </si>
+  <si>
+    <t>Administrator sign up page</t>
+  </si>
+  <si>
+    <t>Administrator form page and input fields validation</t>
+  </si>
+  <si>
+    <t>in progress</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Administrator call API </t>
+  </si>
+  <si>
+    <t>Submit administrator form data to call API and send data to back end</t>
+  </si>
+  <si>
+    <t>Restore registration form data to db</t>
+  </si>
+  <si>
+    <t>provide register api for administrator, receive the form data and insert into database</t>
   </si>
 </sst>
 </file>
@@ -532,7 +580,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -567,9 +615,45 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -588,53 +672,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -950,10 +995,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J59"/>
+  <dimension ref="A1:L59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -973,13 +1018,13 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="2" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="27"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="24"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
@@ -999,61 +1044,61 @@
       </c>
     </row>
     <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="12"/>
+      <c r="B5" s="15"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="19" t="s">
+      <c r="C6" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="19" t="s">
+      <c r="D6" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="19" t="s">
+      <c r="E6" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="19" t="s">
+      <c r="F6" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="G6" s="20" t="s">
+      <c r="G6" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="H6" s="21" t="s">
+      <c r="H6" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="I6" s="17"/>
-      <c r="J6" s="15"/>
+      <c r="I6" s="29"/>
+      <c r="J6" s="27"/>
     </row>
     <row r="7" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="22"/>
-      <c r="B7" s="22" t="s">
+      <c r="A7" s="17"/>
+      <c r="B7" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="22"/>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
-      <c r="F7" s="22"/>
-      <c r="G7" s="23"/>
-      <c r="H7" s="24"/>
-      <c r="I7" s="18"/>
-      <c r="J7" s="16"/>
-    </row>
-    <row r="8" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="C7" s="17"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="33"/>
+      <c r="H7" s="32"/>
+      <c r="I7" s="30"/>
+      <c r="J7" s="28"/>
+    </row>
+    <row r="8" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="11" t="s">
         <v>16</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="28" t="s">
+      <c r="C8" s="12" t="s">
         <v>26</v>
       </c>
       <c r="D8" s="1">
@@ -1065,14 +1110,14 @@
       <c r="F8" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G8" s="28" t="s">
+      <c r="G8" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="H8" s="28" t="s">
+      <c r="H8" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="I8" s="13"/>
-      <c r="J8" s="14"/>
+      <c r="I8" s="25"/>
+      <c r="J8" s="26"/>
     </row>
     <row r="9" spans="1:10" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A9" s="11" t="s">
@@ -1081,7 +1126,7 @@
       <c r="B9" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="28" t="s">
+      <c r="C9" s="12" t="s">
         <v>27</v>
       </c>
       <c r="D9" s="1">
@@ -1093,14 +1138,14 @@
       <c r="F9" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G9" s="28" t="s">
+      <c r="G9" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="H9" s="28" t="s">
+      <c r="H9" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="I9" s="13"/>
-      <c r="J9" s="14"/>
+      <c r="I9" s="25"/>
+      <c r="J9" s="26"/>
     </row>
     <row r="10" spans="1:10" ht="58" x14ac:dyDescent="0.35">
       <c r="A10" s="11" t="s">
@@ -1109,7 +1154,7 @@
       <c r="B10" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="28" t="s">
+      <c r="C10" s="12" t="s">
         <v>33</v>
       </c>
       <c r="D10" s="1">
@@ -1121,10 +1166,10 @@
       <c r="F10" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G10" s="28" t="s">
+      <c r="G10" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="H10" s="28" t="s">
+      <c r="H10" s="12" t="s">
         <v>74</v>
       </c>
       <c r="J10" s="5"/>
@@ -1136,7 +1181,7 @@
       <c r="B11" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="28" t="s">
+      <c r="C11" s="12" t="s">
         <v>37</v>
       </c>
       <c r="D11" s="1">
@@ -1148,10 +1193,10 @@
       <c r="F11" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G11" s="28" t="s">
+      <c r="G11" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="H11" s="28" t="s">
+      <c r="H11" s="12" t="s">
         <v>76</v>
       </c>
       <c r="J11" s="5"/>
@@ -1163,7 +1208,7 @@
       <c r="B12" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="28" t="s">
+      <c r="C12" s="12" t="s">
         <v>34</v>
       </c>
       <c r="D12" s="1">
@@ -1175,10 +1220,10 @@
       <c r="F12" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G12" s="28" t="s">
+      <c r="G12" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="H12" s="28" t="s">
+      <c r="H12" s="12" t="s">
         <v>41</v>
       </c>
       <c r="J12" s="5"/>
@@ -1190,7 +1235,7 @@
       <c r="B13" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="28" t="s">
+      <c r="C13" s="12" t="s">
         <v>35</v>
       </c>
       <c r="D13" s="1">
@@ -1202,10 +1247,10 @@
       <c r="F13" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G13" s="28" t="s">
+      <c r="G13" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="H13" s="28" t="s">
+      <c r="H13" s="12" t="s">
         <v>43</v>
       </c>
       <c r="J13" s="5"/>
@@ -1217,7 +1262,7 @@
       <c r="B14" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C14" s="28" t="s">
+      <c r="C14" s="12" t="s">
         <v>44</v>
       </c>
       <c r="D14" s="1">
@@ -1229,10 +1274,10 @@
       <c r="F14" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G14" s="28" t="s">
+      <c r="G14" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="H14" s="28" t="s">
+      <c r="H14" s="12" t="s">
         <v>75</v>
       </c>
       <c r="J14" s="5"/>
@@ -1244,7 +1289,7 @@
       <c r="B15" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C15" s="28" t="s">
+      <c r="C15" s="12" t="s">
         <v>36</v>
       </c>
       <c r="D15" s="1">
@@ -1256,10 +1301,10 @@
       <c r="F15" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G15" s="28" t="s">
+      <c r="G15" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="H15" s="28" t="s">
+      <c r="H15" s="12" t="s">
         <v>47</v>
       </c>
       <c r="J15" s="5"/>
@@ -1271,7 +1316,7 @@
       <c r="B16" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="28" t="s">
+      <c r="C16" s="12" t="s">
         <v>49</v>
       </c>
       <c r="D16" s="1">
@@ -1283,10 +1328,10 @@
       <c r="F16" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G16" s="28" t="s">
+      <c r="G16" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="H16" s="28" t="s">
+      <c r="H16" s="12" t="s">
         <v>50</v>
       </c>
       <c r="J16" s="5"/>
@@ -1305,47 +1350,51 @@
       <c r="J19" s="5"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A20" s="12" t="s">
+      <c r="A20" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B20" s="12"/>
+      <c r="B20" s="15"/>
     </row>
     <row r="21" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="6"/>
       <c r="J21" s="5"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A22" s="19" t="s">
+      <c r="A22" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="B22" s="19" t="s">
+      <c r="B22" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="C22" s="19" t="s">
+      <c r="C22" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="D22" s="20" t="s">
+      <c r="D22" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="E22" s="29"/>
-      <c r="F22" s="19" t="s">
+      <c r="E22" s="19"/>
+      <c r="F22" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="G22" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="G22" s="28"/>
-      <c r="H22" s="28"/>
+      <c r="H22" s="16" t="s">
+        <v>78</v>
+      </c>
       <c r="J22" s="5"/>
     </row>
     <row r="23" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="22"/>
-      <c r="B23" s="22" t="s">
+      <c r="A23" s="17"/>
+      <c r="B23" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C23" s="22"/>
-      <c r="D23" s="30"/>
-      <c r="E23" s="31"/>
-      <c r="F23" s="22"/>
-      <c r="G23" s="28"/>
-      <c r="H23" s="28"/>
+      <c r="C23" s="17"/>
+      <c r="D23" s="20"/>
+      <c r="E23" s="21"/>
+      <c r="F23" s="17"/>
+      <c r="G23" s="17"/>
+      <c r="H23" s="17"/>
       <c r="J23" s="5"/>
     </row>
     <row r="24" spans="1:10" ht="26.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1355,40 +1404,40 @@
       <c r="B24" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="C24" s="28" t="s">
+      <c r="C24" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="D24" s="33" t="s">
+      <c r="D24" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="E24" s="33"/>
+      <c r="E24" s="14"/>
       <c r="F24" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G24" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G24" s="28"/>
-      <c r="H24" s="28"/>
-      <c r="J24" s="32"/>
     </row>
     <row r="25" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B25" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="C25" s="28" t="s">
+      <c r="C25" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="D25" s="33" t="s">
+      <c r="D25" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="E25" s="33"/>
+      <c r="E25" s="14"/>
       <c r="F25" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G25" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G25" s="28"/>
-      <c r="H25" s="28"/>
-      <c r="J25" s="32"/>
     </row>
     <row r="26" spans="1:10" ht="49" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="11" t="s">
@@ -1397,18 +1446,19 @@
       <c r="B26" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="C26" s="28" t="s">
+      <c r="C26" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="D26" s="33" t="s">
+      <c r="D26" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="E26" s="33"/>
+      <c r="E26" s="14"/>
       <c r="F26" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="G26" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G26" s="28"/>
-      <c r="H26" s="28"/>
     </row>
     <row r="27" spans="1:10" ht="48.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="11" t="s">
@@ -1417,18 +1467,19 @@
       <c r="B27" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="C27" s="28" t="s">
+      <c r="C27" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="D27" s="33" t="s">
+      <c r="D27" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="E27" s="33"/>
+      <c r="E27" s="14"/>
       <c r="F27" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="G27" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G27" s="28"/>
-      <c r="H27" s="28"/>
       <c r="J27" s="5"/>
     </row>
     <row r="28" spans="1:10" ht="78" customHeight="1" x14ac:dyDescent="0.35">
@@ -1438,18 +1489,19 @@
       <c r="B28" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="C28" s="28" t="s">
+      <c r="C28" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="D28" s="33" t="s">
+      <c r="D28" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="E28" s="33"/>
+      <c r="E28" s="14"/>
       <c r="F28" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G28" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G28" s="28"/>
-      <c r="H28" s="28"/>
       <c r="J28" s="5"/>
     </row>
     <row r="29" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.35">
@@ -1459,103 +1511,209 @@
       <c r="B29" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="C29" s="34" t="s">
+      <c r="C29" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="D29" s="33" t="s">
+      <c r="D29" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="E29" s="33"/>
+      <c r="E29" s="14"/>
       <c r="F29" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="G29" s="1" t="s">
         <v>23</v>
       </c>
       <c r="J29" s="5"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A30" s="6"/>
-      <c r="D30" s="33"/>
-      <c r="E30" s="33"/>
+      <c r="D30" s="14"/>
+      <c r="E30" s="14"/>
       <c r="J30" s="5"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A31" s="6"/>
-      <c r="D31" s="33"/>
-      <c r="E31" s="33"/>
+      <c r="D31" s="14"/>
+      <c r="E31" s="14"/>
       <c r="J31" s="5"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A32" s="6"/>
-      <c r="D32" s="33"/>
-      <c r="E32" s="33"/>
+      <c r="D32" s="14"/>
+      <c r="E32" s="14"/>
       <c r="J32" s="5"/>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A33" s="6"/>
-      <c r="D33" s="33"/>
-      <c r="E33" s="33"/>
+      <c r="D33" s="14"/>
+      <c r="E33" s="14"/>
       <c r="J33" s="5"/>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A34" s="12" t="s">
+    <row r="34" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A34" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="B34" s="12"/>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A35" s="6"/>
-      <c r="D35" s="33"/>
-      <c r="E35" s="33"/>
-      <c r="J35" s="5"/>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A36" s="6"/>
-      <c r="J36" s="5"/>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A37" s="6"/>
-      <c r="J37" s="5"/>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A38" s="6"/>
-      <c r="J38" s="5"/>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A39" s="6"/>
-      <c r="J39" s="5"/>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A40" s="6"/>
-      <c r="J40" s="5"/>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A41" s="6"/>
-      <c r="J41" s="5"/>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A42" s="6"/>
-      <c r="J42" s="5"/>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A43" s="6"/>
-      <c r="J43" s="5"/>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B34" s="15"/>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A35" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="B35" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="C35" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="D35" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="E35" s="19"/>
+      <c r="F35" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="G35" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="H35" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="K35" s="14"/>
+      <c r="L35" s="14"/>
+    </row>
+    <row r="36" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A36" s="17"/>
+      <c r="B36" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="C36" s="17"/>
+      <c r="D36" s="20"/>
+      <c r="E36" s="21"/>
+      <c r="F36" s="17"/>
+      <c r="G36" s="17"/>
+      <c r="H36" s="17"/>
+    </row>
+    <row r="37" spans="1:12" ht="41.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B37" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="C37" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="D37" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="E37" s="14"/>
+      <c r="F37" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" ht="52.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B38" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="C38" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="D38" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="E38" s="14"/>
+      <c r="F38" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" ht="70" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B39" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="C39" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="D39" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="E39" s="14"/>
+      <c r="F39" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A40" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D40" s="14"/>
+      <c r="E40" s="14"/>
+      <c r="H40" s="6"/>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A41" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D41" s="14"/>
+      <c r="E41" s="14"/>
+      <c r="H41" s="6"/>
+    </row>
+    <row r="42" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D42" s="14"/>
+      <c r="E42" s="14"/>
+      <c r="H42" s="6"/>
+    </row>
+    <row r="43" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D43" s="14"/>
+      <c r="E43" s="14"/>
+      <c r="H43" s="6"/>
+    </row>
+    <row r="44" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="6"/>
+      <c r="D44" s="14"/>
+      <c r="E44" s="14"/>
       <c r="J44" s="5"/>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A45" s="6"/>
+      <c r="D45" s="14"/>
+      <c r="E45" s="14"/>
       <c r="J45" s="5"/>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A46" s="6"/>
+      <c r="D46" s="14"/>
+      <c r="E46" s="14"/>
       <c r="J46" s="5"/>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A47" s="6"/>
+      <c r="D47" s="14"/>
+      <c r="E47" s="14"/>
       <c r="J47" s="5"/>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A48" s="6"/>
       <c r="J48" s="5"/>
     </row>
@@ -1612,30 +1770,28 @@
       <c r="J59" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="32">
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="F22:F23"/>
-    <mergeCell ref="D22:E23"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="A5:B5"/>
+  <mergeCells count="52">
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="D47:E47"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="K35:L35"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="G22:G23"/>
+    <mergeCell ref="H22:H23"/>
+    <mergeCell ref="A35:A36"/>
+    <mergeCell ref="B35:B36"/>
+    <mergeCell ref="C35:C36"/>
+    <mergeCell ref="D35:E36"/>
+    <mergeCell ref="F35:F36"/>
+    <mergeCell ref="G35:G36"/>
+    <mergeCell ref="H35:H36"/>
     <mergeCell ref="I8:I9"/>
     <mergeCell ref="J8:J9"/>
     <mergeCell ref="A6:A7"/>
@@ -1645,6 +1801,28 @@
     <mergeCell ref="G6:G7"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="F22:F23"/>
+    <mergeCell ref="D22:E23"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="D33:E33"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>